<commit_message>
Added choropleth map feature for districts
</commit_message>
<xml_diff>
--- a/assets/RLFS_2022_Data_clean.xlsx
+++ b/assets/RLFS_2022_Data_clean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20415" windowHeight="7695" firstSheet="3" activeTab="8"/>
+    <workbookView windowWidth="20415" windowHeight="7695" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="table_names" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
   <si>
     <t>Table 0: Summary table of youth between 16-30</t>
   </si>
@@ -254,19 +254,13 @@
     <t>no education</t>
   </si>
   <si>
-    <t>district</t>
+    <t>Districts</t>
   </si>
   <si>
     <t>rate</t>
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lon</t>
   </si>
   <si>
     <t>Nyarugenge</t>
@@ -365,12 +359,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="###0"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -456,21 +450,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,34 +474,16 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -532,14 +503,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,8 +524,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -562,7 +541,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -575,10 +568,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -603,43 +597,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +621,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,7 +633,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +663,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,7 +699,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,73 +771,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,36 +826,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -910,6 +874,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -917,6 +896,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -934,145 +928,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1085,13 +1079,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1103,9 +1100,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1115,9 +1109,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1133,7 +1127,7 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1145,9 +1139,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="37" fontId="6" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1166,7 +1157,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="7" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1178,7 +1169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1533,104 +1524,104 @@
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelCol="7"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
       <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="39"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="40"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1665,8 +1656,8 @@
   <sheetPr/>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1686,522 +1677,398 @@
       <c r="C1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>40232</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="4">
+        <v>21.2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>78762</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B4" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>52090</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21.3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>24406</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20.9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>24542</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="C7" s="5">
+        <v>23747</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="4">
+        <v>19.7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>27643</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="C9" s="5">
+        <v>30001</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="4">
         <v>20.5</v>
       </c>
-      <c r="C2" s="4">
-        <v>40232</v>
-      </c>
-      <c r="D2" s="5">
-        <v>-1.9567</v>
-      </c>
-      <c r="E2" s="5">
-        <v>30.0636</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="3">
-        <v>21.2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>78762</v>
-      </c>
-      <c r="D3" s="5">
-        <v>-1.8898</v>
-      </c>
-      <c r="E3" s="5">
-        <v>30.1127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="C10" s="5">
+        <v>29311</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="4">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5">
+        <v>34385</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="4">
+        <v>22.1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>28817</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="4">
+        <v>22.7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>30047</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="4">
+        <v>19.9</v>
+      </c>
+      <c r="C14" s="5">
+        <v>22933</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="4">
+        <v>19.8</v>
+      </c>
+      <c r="C15" s="5">
+        <v>29533</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="4">
+        <v>19.1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>22289</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="4">
+        <v>17.6</v>
+      </c>
+      <c r="C17" s="5">
+        <v>17682</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="4">
+        <v>21.9</v>
+      </c>
+      <c r="C18" s="5">
+        <v>26898</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="4">
+        <v>25.8</v>
+      </c>
+      <c r="C19" s="5">
+        <v>21556</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>27777</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="4">
+        <v>16.9</v>
+      </c>
+      <c r="C21" s="5">
+        <v>24370</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="4">
+        <v>18.7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>36034</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="4">
+        <v>24.3</v>
+      </c>
+      <c r="C23" s="5">
+        <v>30532</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="4">
         <v>20.7</v>
       </c>
-      <c r="C4" s="4">
-        <v>52090</v>
-      </c>
-      <c r="D4" s="5">
-        <v>-1.9689</v>
-      </c>
-      <c r="E4" s="5">
-        <v>30.0925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="3">
-        <v>21.3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>24406</v>
-      </c>
-      <c r="D5" s="5">
-        <v>-2.3433</v>
-      </c>
-      <c r="E5" s="5">
-        <v>29.743</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="3">
-        <v>20.9</v>
-      </c>
-      <c r="C6" s="4">
-        <v>24542</v>
-      </c>
-      <c r="D6" s="5">
-        <v>-2.5217</v>
-      </c>
-      <c r="E6" s="5">
-        <v>29.5391</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="3">
-        <v>21.9</v>
-      </c>
-      <c r="C7" s="4">
-        <v>23747</v>
-      </c>
-      <c r="D7" s="5">
-        <v>-2.589</v>
-      </c>
-      <c r="E7" s="5">
-        <v>29.4918</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="3">
-        <v>19.7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>27643</v>
-      </c>
-      <c r="D8" s="5">
-        <v>-2.6022</v>
-      </c>
-      <c r="E8" s="5">
-        <v>29.7345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="3">
-        <v>21.9</v>
-      </c>
-      <c r="C9" s="4">
-        <v>30001</v>
-      </c>
-      <c r="D9" s="5">
-        <v>-2.453855</v>
-      </c>
-      <c r="E9" s="5">
-        <v>29.464359</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="C10" s="4">
-        <v>29311</v>
-      </c>
-      <c r="D10" s="5">
-        <v>-1.973</v>
-      </c>
-      <c r="E10" s="5">
-        <v>29.7308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="3">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4">
-        <v>34385</v>
-      </c>
-      <c r="D11" s="5">
-        <v>-2.1618</v>
-      </c>
-      <c r="E11" s="5">
-        <v>29.729</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="3">
-        <v>22.1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>28817</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-2.0108</v>
-      </c>
-      <c r="E12" s="5">
-        <v>29.9929</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="3">
-        <v>22.7</v>
-      </c>
-      <c r="C13" s="4">
-        <v>30047</v>
-      </c>
-      <c r="D13" s="5">
-        <v>-2.17897</v>
-      </c>
-      <c r="E13" s="5">
-        <v>29.371491</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="3">
-        <v>19.9</v>
-      </c>
-      <c r="C14" s="4">
-        <v>22933</v>
-      </c>
-      <c r="D14" s="5">
-        <v>-2.5044</v>
-      </c>
-      <c r="E14" s="5">
-        <v>29.1499</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="3">
-        <v>19.8</v>
-      </c>
-      <c r="C15" s="4">
-        <v>29533</v>
-      </c>
-      <c r="D15" s="5">
-        <v>-1.689292</v>
-      </c>
-      <c r="E15" s="5">
-        <v>29.293087</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="3">
-        <v>19.1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>22289</v>
-      </c>
-      <c r="D16" s="5">
-        <v>-1.7162</v>
-      </c>
-      <c r="E16" s="5">
-        <v>29.573</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="3">
-        <v>17.6</v>
-      </c>
-      <c r="C17" s="4">
-        <v>17682</v>
-      </c>
-      <c r="D17" s="5">
-        <v>-2.0886</v>
-      </c>
-      <c r="E17" s="5">
-        <v>29.4234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="3">
-        <v>21.9</v>
-      </c>
-      <c r="C18" s="4">
-        <v>26898</v>
-      </c>
-      <c r="D18" s="5">
-        <v>-2.5285</v>
-      </c>
-      <c r="E18" s="5">
-        <v>28.9088</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="3">
-        <v>25.8</v>
-      </c>
-      <c r="C19" s="4">
-        <v>21556</v>
-      </c>
-      <c r="D19" s="5">
-        <v>-2.4928</v>
-      </c>
-      <c r="E19" s="5">
-        <v>29.3536</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="3">
-        <v>23.2</v>
-      </c>
-      <c r="C20" s="4">
-        <v>27777</v>
-      </c>
-      <c r="D20" s="5">
-        <v>-1.973</v>
-      </c>
-      <c r="E20" s="5">
-        <v>29.7308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="3">
-        <v>16.9</v>
-      </c>
-      <c r="C21" s="4">
-        <v>24370</v>
-      </c>
-      <c r="D21" s="5">
-        <v>-1.7483</v>
-      </c>
-      <c r="E21" s="5">
-        <v>29.7626</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="3">
-        <v>18.7</v>
-      </c>
-      <c r="C22" s="4">
-        <v>36034</v>
-      </c>
-      <c r="D22" s="5">
-        <v>-1.5047</v>
-      </c>
-      <c r="E22" s="5">
-        <v>29.631</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
+      <c r="C24" s="5">
+        <v>35455</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="3">
-        <v>24.3</v>
-      </c>
-      <c r="C23" s="4">
-        <v>30532</v>
-      </c>
-      <c r="D23" s="5">
-        <v>-1.5808</v>
-      </c>
-      <c r="E23" s="5">
-        <v>29.7369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2" t="s">
+      <c r="B25" s="4">
+        <v>19.6</v>
+      </c>
+      <c r="C25" s="5">
+        <v>30188</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="3">
-        <v>20.7</v>
-      </c>
-      <c r="C24" s="4">
-        <v>35455</v>
-      </c>
-      <c r="D24" s="5">
-        <v>-1.8897</v>
-      </c>
-      <c r="E24" s="5">
-        <v>29.801</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
+      <c r="B26" s="4">
+        <v>19.3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>32707</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="3">
-        <v>19.6</v>
-      </c>
-      <c r="C25" s="4">
-        <v>30188</v>
-      </c>
-      <c r="D25" s="5">
-        <v>-1.9406</v>
-      </c>
-      <c r="E25" s="5">
-        <v>30.4381</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
+      <c r="B27" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>42392</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="3">
-        <v>19.3</v>
-      </c>
-      <c r="C26" s="4">
-        <v>32707</v>
-      </c>
-      <c r="D26" s="5">
-        <v>-1.3146</v>
-      </c>
-      <c r="E26" s="5">
-        <v>30.3724</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="C28" s="5">
+        <v>24914</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="3">
-        <v>22.5</v>
-      </c>
-      <c r="C27" s="4">
-        <v>42392</v>
-      </c>
-      <c r="D27" s="5">
-        <v>-1.677</v>
-      </c>
-      <c r="E27" s="5">
-        <v>30.4346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
+      <c r="B29" s="4">
+        <v>16.1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>19706</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="3">
-        <v>15.9</v>
-      </c>
-      <c r="C28" s="4">
-        <v>24914</v>
-      </c>
-      <c r="D28" s="5">
-        <v>-1.851</v>
-      </c>
-      <c r="E28" s="5">
-        <v>30.651</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="4">
+        <v>15.6</v>
+      </c>
+      <c r="C30" s="5">
+        <v>19372</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="3">
-        <v>16.1</v>
-      </c>
-      <c r="C29" s="4">
-        <v>19706</v>
-      </c>
-      <c r="D29" s="5">
-        <v>-2.263273</v>
-      </c>
-      <c r="E29" s="5">
-        <v>30.641561</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="3">
-        <v>15.6</v>
-      </c>
-      <c r="C30" s="4">
-        <v>19372</v>
-      </c>
-      <c r="D30" s="5">
-        <v>-2.15535</v>
-      </c>
-      <c r="E30" s="5">
-        <v>30.56833</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>23.7</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>28625</v>
       </c>
-      <c r="D31" s="5">
-        <v>-2.1597</v>
-      </c>
-      <c r="E31" s="5">
-        <v>30.1469</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2251,163 +2118,163 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="34">
         <v>466370</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>25.6</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="34">
         <v>215337</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="34">
         <v>251034</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>110663</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <v>355707</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="34">
         <v>134737</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>21.2</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>70892</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>63846</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>11830</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>122908</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="34">
         <v>48917</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>22.9</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>64996</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>84689</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>18464</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>131222</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="34">
         <v>48917</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>27.1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>64996</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>84689</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>18464</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>131222</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="34">
         <v>109142</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>39.4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>50455</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>58688</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>48599</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>60543</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="34">
         <v>25100</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>32.4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>10185</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>14915</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>17972</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <v>7128</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="34">
         <v>1217890</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>35.6</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>504465</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>713425</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>79048</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <v>1138842</v>
       </c>
     </row>
@@ -2453,27 +2320,27 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="29">
         <v>7963586</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <v>3753869</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <v>4209718</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>1637017</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="29">
         <v>6326569</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="13">
@@ -2491,11 +2358,11 @@
       <c r="F3" s="13">
         <v>727246</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="13">
@@ -2513,14 +2380,14 @@
       <c r="F4" s="13">
         <v>5599323</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="13">
@@ -2538,11 +2405,11 @@
       <c r="F5" s="13">
         <v>2156840</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="13">
@@ -2560,11 +2427,11 @@
       <c r="F6" s="13">
         <v>501309</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="13">
@@ -2582,11 +2449,11 @@
       <c r="F7" s="13">
         <v>355887</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="13">
@@ -2606,12 +2473,12 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="33"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2654,138 +2521,138 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="26">
         <v>362908</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>168886</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="26">
         <v>194022</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="26">
         <v>11302</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>5340</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="26">
         <v>5962</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="26">
         <v>23473</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>9934</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>13539</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>82386</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>37160</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>45226</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>139032</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>62822</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>76210</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>48203</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>29114</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>19089</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="26">
         <v>15852</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <v>8353</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <v>7499</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>18211</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>3510</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>14701</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>15707</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <v>5921</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="26">
         <v>9786</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2823,108 +2690,108 @@
         <v>38</v>
       </c>
       <c r="G1" s="8"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>1217890</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>0.342</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>79048</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>0.022</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>1138842</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>0.32</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>800000</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>0.225</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>25000</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>0.007</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>775000</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>0.218</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>2017890</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>0.567</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>104048</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>0.029</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>1913842</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>0.538</v>
       </c>
     </row>
@@ -3114,13 +2981,13 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3421,7 +3288,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="11">
@@ -3587,8 +3454,8 @@
   <sheetPr/>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15"/>
@@ -3635,13 +3502,13 @@
       <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>1217890</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>504465</v>
       </c>
       <c r="D2" s="7">
@@ -3664,13 +3531,13 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>365555</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>191419</v>
       </c>
       <c r="D3" s="7">
@@ -3693,7 +3560,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B4" s="7">
@@ -3722,13 +3589,13 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>419187</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>133231</v>
       </c>
       <c r="D5" s="7">
@@ -3751,13 +3618,13 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>455861</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>228486</v>
       </c>
       <c r="D6" s="7">
@@ -3780,13 +3647,13 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>440354</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>153952</v>
       </c>
       <c r="D7" s="7">
@@ -3809,13 +3676,13 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>117564</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>37160</v>
       </c>
       <c r="D8" s="7">
@@ -3838,13 +3705,13 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>176237</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>73021</v>
       </c>
       <c r="D9" s="7">
@@ -3867,13 +3734,13 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="7">
         <v>27874</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>11845</v>
       </c>
       <c r="D10" s="7">

</xml_diff>